<commit_message>
Changes forward position names: RF/LF to RS/LS. Squad updates
</commit_message>
<xml_diff>
--- a/Source/EuroManager.WorldSimulator.Tests.Manual/Data.xlsx
+++ b/Source/EuroManager.WorldSimulator.Tests.Manual/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="World" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="153">
   <si>
     <t>Name</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Strategy</t>
   </si>
   <si>
-    <t>Bilbao</t>
-  </si>
-  <si>
     <t>Athletic Bilbao</t>
   </si>
   <si>
@@ -160,6 +157,327 @@
   </si>
   <si>
     <t>CAM</t>
+  </si>
+  <si>
+    <t>Athletic</t>
+  </si>
+  <si>
+    <t>Arsenal</t>
+  </si>
+  <si>
+    <t>Arsenal FC</t>
+  </si>
+  <si>
+    <t>Aston Villa</t>
+  </si>
+  <si>
+    <t>Chelsea</t>
+  </si>
+  <si>
+    <t>Chelsea FC</t>
+  </si>
+  <si>
+    <t>Everton</t>
+  </si>
+  <si>
+    <t>Everton FC</t>
+  </si>
+  <si>
+    <t>Fulham</t>
+  </si>
+  <si>
+    <t>Fulham FC</t>
+  </si>
+  <si>
+    <t>Liverpool</t>
+  </si>
+  <si>
+    <t>Liverpool FC</t>
+  </si>
+  <si>
+    <t>Man City</t>
+  </si>
+  <si>
+    <t>Manchester City</t>
+  </si>
+  <si>
+    <t>Man Utd</t>
+  </si>
+  <si>
+    <t>Manchester United</t>
+  </si>
+  <si>
+    <t>Norwich</t>
+  </si>
+  <si>
+    <t>Norwich City</t>
+  </si>
+  <si>
+    <t>QPR</t>
+  </si>
+  <si>
+    <t>Queens Park Rangers</t>
+  </si>
+  <si>
+    <t>Reading</t>
+  </si>
+  <si>
+    <t>Reading FC</t>
+  </si>
+  <si>
+    <t>Southampton</t>
+  </si>
+  <si>
+    <t>Southampton FC</t>
+  </si>
+  <si>
+    <t>Tottenham</t>
+  </si>
+  <si>
+    <t>Tottenham Hotspur</t>
+  </si>
+  <si>
+    <t>Stoke</t>
+  </si>
+  <si>
+    <t>Stoke City</t>
+  </si>
+  <si>
+    <t>Sunderland</t>
+  </si>
+  <si>
+    <t>Sunderland AFC</t>
+  </si>
+  <si>
+    <t>Swansea</t>
+  </si>
+  <si>
+    <t>Swansea City</t>
+  </si>
+  <si>
+    <t>West Brom</t>
+  </si>
+  <si>
+    <t>West Bromwich Albion</t>
+  </si>
+  <si>
+    <t>West Ham</t>
+  </si>
+  <si>
+    <t>West Ham United</t>
+  </si>
+  <si>
+    <t>Wigan</t>
+  </si>
+  <si>
+    <t>Wigan Athletic</t>
+  </si>
+  <si>
+    <t>Szczesny</t>
+  </si>
+  <si>
+    <t>Sagna</t>
+  </si>
+  <si>
+    <t>RCB</t>
+  </si>
+  <si>
+    <t>Koscielny</t>
+  </si>
+  <si>
+    <t>LCB</t>
+  </si>
+  <si>
+    <t>Vermaelen</t>
+  </si>
+  <si>
+    <t>Gibbs</t>
+  </si>
+  <si>
+    <t>RCM</t>
+  </si>
+  <si>
+    <t>LCM</t>
+  </si>
+  <si>
+    <t>LW</t>
+  </si>
+  <si>
+    <t>Podolski</t>
+  </si>
+  <si>
+    <t>Walcott</t>
+  </si>
+  <si>
+    <t>Giroud</t>
+  </si>
+  <si>
+    <t>Wilshere</t>
+  </si>
+  <si>
+    <t>Given</t>
+  </si>
+  <si>
+    <t>Lichaj</t>
+  </si>
+  <si>
+    <t>Vlaar</t>
+  </si>
+  <si>
+    <t>Clark</t>
+  </si>
+  <si>
+    <t>Bennett</t>
+  </si>
+  <si>
+    <t>Herd</t>
+  </si>
+  <si>
+    <t>CM</t>
+  </si>
+  <si>
+    <t>El Ahmadi</t>
+  </si>
+  <si>
+    <t>Bannan</t>
+  </si>
+  <si>
+    <t>Ireland</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>Bent</t>
+  </si>
+  <si>
+    <t>LS</t>
+  </si>
+  <si>
+    <t>Agbonlahor</t>
+  </si>
+  <si>
+    <t>Cech</t>
+  </si>
+  <si>
+    <t>Ivanovic</t>
+  </si>
+  <si>
+    <t>David Luiz</t>
+  </si>
+  <si>
+    <t>Santi Cazorla</t>
+  </si>
+  <si>
+    <t>Mikel Arteta</t>
+  </si>
+  <si>
+    <t>Terry</t>
+  </si>
+  <si>
+    <t>A. Cole</t>
+  </si>
+  <si>
+    <t>RDM</t>
+  </si>
+  <si>
+    <t>Ramires</t>
+  </si>
+  <si>
+    <t>Lampard</t>
+  </si>
+  <si>
+    <t>Oscar</t>
+  </si>
+  <si>
+    <t>Hazard</t>
+  </si>
+  <si>
+    <t>Mata</t>
+  </si>
+  <si>
+    <t>F. Torres</t>
+  </si>
+  <si>
+    <t>Howard</t>
+  </si>
+  <si>
+    <t>Hibbert</t>
+  </si>
+  <si>
+    <t>Jagielka</t>
+  </si>
+  <si>
+    <t>Heitinga</t>
+  </si>
+  <si>
+    <t>Baines</t>
+  </si>
+  <si>
+    <t>RWB</t>
+  </si>
+  <si>
+    <t>LWB</t>
+  </si>
+  <si>
+    <t>RM</t>
+  </si>
+  <si>
+    <t>Osman</t>
+  </si>
+  <si>
+    <t>P. Neville</t>
+  </si>
+  <si>
+    <t>Gibson</t>
+  </si>
+  <si>
+    <t>LM</t>
+  </si>
+  <si>
+    <t>Pienaar</t>
+  </si>
+  <si>
+    <t>Fellaini</t>
+  </si>
+  <si>
+    <t>Jelavic</t>
+  </si>
+  <si>
+    <t>Schwarzer</t>
+  </si>
+  <si>
+    <t>Riether</t>
+  </si>
+  <si>
+    <t>Hughes</t>
+  </si>
+  <si>
+    <t>Hangeland</t>
+  </si>
+  <si>
+    <t>Riise</t>
+  </si>
+  <si>
+    <t>Sidwell</t>
+  </si>
+  <si>
+    <t>LDM</t>
+  </si>
+  <si>
+    <t>M. Diarra</t>
+  </si>
+  <si>
+    <t>Duff</t>
+  </si>
+  <si>
+    <t>Richardson</t>
+  </si>
+  <si>
+    <t>B. Ruiz</t>
+  </si>
+  <si>
+    <t>Berbatov</t>
   </si>
 </sst>
 </file>
@@ -247,8 +565,12 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:D6" totalsRowShown="0">
-  <autoFilter ref="A1:D6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:D25" totalsRowShown="0">
+  <autoFilter ref="A1:D25"/>
+  <sortState ref="A2:D25">
+    <sortCondition ref="C2:C25"/>
+    <sortCondition ref="B2:B25"/>
+  </sortState>
   <tableColumns count="4">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
@@ -260,12 +582,19 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="A1:F8" totalsRowShown="0">
-  <autoFilter ref="A1:F8"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Name"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="A1:G63" totalsRowShown="0">
+  <autoFilter ref="A1:G63"/>
+  <sortState ref="A2:G63">
+    <sortCondition ref="A2:A63"/>
+    <sortCondition ref="B2:B63"/>
+    <sortCondition ref="C2:C63" customList="GK,RWB,RB,RCB,CB,LCB,LB,LWB,RDM,CDM,LDM,RM,RCM,CM,LCM,LM,RAM,CAM,LAM,RW,LW,CF,RS,LS,ST"/>
+    <sortCondition ref="D2:D63"/>
+  </sortState>
+  <tableColumns count="7">
+    <tableColumn id="7" name="Division"/>
     <tableColumn id="2" name="Club"/>
     <tableColumn id="3" name="Position"/>
+    <tableColumn id="1" name="Name"/>
     <tableColumn id="4" name="Defending"/>
     <tableColumn id="5" name="Attacking"/>
     <tableColumn id="6" name="Form"/>
@@ -631,18 +960,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -677,21 +1006,21 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -699,13 +1028,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -721,10 +1050,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -743,7 +1072,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
@@ -751,69 +1080,335 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
         <v>39</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" t="s">
         <v>43</v>
       </c>
-      <c r="B6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
+      <c r="D25" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -826,183 +1421,1472 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="6" width="5.5546875" customWidth="1"/>
+    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" customWidth="1"/>
+    <col min="4" max="4" width="21.109375" customWidth="1"/>
+    <col min="5" max="9" width="5.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
         <v>19</v>
       </c>
-      <c r="C1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="D2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2">
+        <v>80</v>
+      </c>
+      <c r="F2">
+        <v>50</v>
+      </c>
+      <c r="G2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3">
+        <v>83</v>
+      </c>
+      <c r="F3">
+        <v>78</v>
+      </c>
+      <c r="G3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4">
+        <v>81</v>
+      </c>
+      <c r="F4">
+        <v>68</v>
+      </c>
+      <c r="G4">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5">
+        <v>82</v>
+      </c>
+      <c r="F5">
+        <v>62</v>
+      </c>
+      <c r="G5">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6">
+        <v>76</v>
+      </c>
+      <c r="F6">
+        <v>72</v>
+      </c>
+      <c r="G6">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E7">
+        <v>75</v>
+      </c>
+      <c r="F7">
+        <v>81</v>
+      </c>
+      <c r="G7">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8">
+        <v>70</v>
+      </c>
+      <c r="F8">
+        <v>82</v>
+      </c>
+      <c r="G8">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E9">
+        <v>69</v>
+      </c>
+      <c r="F9">
+        <v>84</v>
+      </c>
+      <c r="G9">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>95</v>
+      </c>
+      <c r="E10">
+        <v>63</v>
+      </c>
+      <c r="F10">
+        <v>81</v>
+      </c>
+      <c r="G10">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E11">
+        <v>65</v>
+      </c>
+      <c r="F11">
+        <v>83</v>
+      </c>
+      <c r="G11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
+        <v>96</v>
+      </c>
+      <c r="E12">
+        <v>68</v>
+      </c>
+      <c r="F12">
+        <v>80</v>
+      </c>
+      <c r="G12">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" t="s">
+        <v>98</v>
+      </c>
+      <c r="E13">
+        <v>80</v>
+      </c>
+      <c r="F13">
+        <v>50</v>
+      </c>
+      <c r="G13">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s">
+        <v>99</v>
+      </c>
+      <c r="E14">
+        <v>70</v>
+      </c>
+      <c r="F14">
+        <v>65</v>
+      </c>
+      <c r="G14">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D15" t="s">
+        <v>100</v>
+      </c>
+      <c r="E15">
+        <v>76</v>
+      </c>
+      <c r="F15">
+        <v>62</v>
+      </c>
+      <c r="G15">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" t="s">
+        <v>101</v>
+      </c>
+      <c r="E16">
+        <v>74</v>
+      </c>
+      <c r="F16">
+        <v>65</v>
+      </c>
+      <c r="G16">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" t="s">
+        <v>102</v>
+      </c>
+      <c r="E17">
+        <v>66</v>
+      </c>
+      <c r="F17">
+        <v>71</v>
+      </c>
+      <c r="G17">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" t="s">
+        <v>103</v>
+      </c>
+      <c r="E18">
+        <v>64</v>
+      </c>
+      <c r="F18">
+        <v>67</v>
+      </c>
+      <c r="G18">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D19" t="s">
+        <v>105</v>
+      </c>
+      <c r="E19">
+        <v>71</v>
+      </c>
+      <c r="F19">
+        <v>75</v>
+      </c>
+      <c r="G19">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20" t="s">
+        <v>106</v>
+      </c>
+      <c r="E20">
+        <v>72</v>
+      </c>
+      <c r="F20">
+        <v>73</v>
+      </c>
+      <c r="G20">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" t="s">
+        <v>107</v>
+      </c>
+      <c r="E21">
+        <v>64</v>
+      </c>
+      <c r="F21">
+        <v>77</v>
+      </c>
+      <c r="G21">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" t="s">
+        <v>108</v>
+      </c>
+      <c r="D22" t="s">
+        <v>109</v>
+      </c>
+      <c r="E22">
+        <v>71</v>
+      </c>
+      <c r="F22">
+        <v>82</v>
+      </c>
+      <c r="G22">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" t="s">
+        <v>110</v>
+      </c>
+      <c r="D23" t="s">
+        <v>111</v>
+      </c>
+      <c r="E23">
+        <v>62</v>
+      </c>
+      <c r="F23">
+        <v>74</v>
+      </c>
+      <c r="G23">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" t="s">
+        <v>112</v>
+      </c>
+      <c r="E24">
+        <v>84</v>
+      </c>
+      <c r="F24">
+        <v>56</v>
+      </c>
+      <c r="G24">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" t="s">
+        <v>131</v>
+      </c>
+      <c r="D25" t="s">
+        <v>113</v>
+      </c>
+      <c r="E25">
+        <v>82</v>
+      </c>
+      <c r="F25">
+        <v>84</v>
+      </c>
+      <c r="G25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" t="s">
+        <v>86</v>
+      </c>
+      <c r="D26" t="s">
+        <v>114</v>
+      </c>
+      <c r="E26">
+        <v>79</v>
+      </c>
+      <c r="F26">
+        <v>76</v>
+      </c>
+      <c r="G26">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" t="s">
+        <v>88</v>
+      </c>
+      <c r="D27" t="s">
+        <v>117</v>
+      </c>
+      <c r="E27">
+        <v>84</v>
+      </c>
+      <c r="F27">
+        <v>70</v>
+      </c>
+      <c r="G27">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" t="s">
+        <v>132</v>
+      </c>
+      <c r="D28" t="s">
+        <v>118</v>
+      </c>
+      <c r="E28">
+        <v>84</v>
+      </c>
+      <c r="F28">
+        <v>80</v>
+      </c>
+      <c r="G28">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" t="s">
+        <v>91</v>
+      </c>
+      <c r="D29" t="s">
+        <v>120</v>
+      </c>
+      <c r="E29">
+        <v>81</v>
+      </c>
+      <c r="F29">
+        <v>76</v>
+      </c>
+      <c r="G29">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" t="s">
+        <v>92</v>
+      </c>
+      <c r="D30" t="s">
+        <v>121</v>
+      </c>
+      <c r="E30">
+        <v>83</v>
+      </c>
+      <c r="F30">
+        <v>86</v>
+      </c>
+      <c r="G30">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" t="s">
+        <v>122</v>
+      </c>
+      <c r="E31">
+        <v>66</v>
+      </c>
+      <c r="F31">
+        <v>82</v>
+      </c>
+      <c r="G31">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" t="s">
+        <v>123</v>
+      </c>
+      <c r="E32">
+        <v>63</v>
+      </c>
+      <c r="F32">
+        <v>87</v>
+      </c>
+      <c r="G32">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" t="s">
+        <v>93</v>
+      </c>
+      <c r="D33" t="s">
+        <v>124</v>
+      </c>
+      <c r="E33">
+        <v>70</v>
+      </c>
+      <c r="F33">
+        <v>86</v>
+      </c>
+      <c r="G33">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D34" t="s">
+        <v>125</v>
+      </c>
+      <c r="E34">
+        <v>62</v>
+      </c>
+      <c r="F34">
+        <v>85</v>
+      </c>
+      <c r="G34">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" t="s">
+        <v>126</v>
+      </c>
+      <c r="E35">
+        <v>81</v>
+      </c>
+      <c r="F35">
+        <v>59</v>
+      </c>
+      <c r="G35">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36" t="s">
+        <v>131</v>
+      </c>
+      <c r="D36" t="s">
+        <v>127</v>
+      </c>
+      <c r="E36">
+        <v>74</v>
+      </c>
+      <c r="F36">
+        <v>72</v>
+      </c>
+      <c r="G36">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37" t="s">
+        <v>86</v>
+      </c>
+      <c r="D37" t="s">
+        <v>128</v>
+      </c>
+      <c r="E37">
+        <v>79</v>
+      </c>
+      <c r="F37">
+        <v>70</v>
+      </c>
+      <c r="G37">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" t="s">
+        <v>88</v>
+      </c>
+      <c r="D38" t="s">
+        <v>129</v>
+      </c>
+      <c r="E38">
+        <v>79</v>
+      </c>
+      <c r="F38">
+        <v>77</v>
+      </c>
+      <c r="G38">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" t="s">
+        <v>52</v>
+      </c>
+      <c r="C39" t="s">
+        <v>132</v>
+      </c>
+      <c r="D39" t="s">
+        <v>130</v>
+      </c>
+      <c r="E39">
+        <v>80</v>
+      </c>
+      <c r="F39">
+        <v>78</v>
+      </c>
+      <c r="G39">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>52</v>
+      </c>
+      <c r="C40" t="s">
+        <v>133</v>
+      </c>
+      <c r="D40" t="s">
+        <v>134</v>
+      </c>
+      <c r="E40">
+        <v>71</v>
+      </c>
+      <c r="F40">
+        <v>78</v>
+      </c>
+      <c r="G40">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41" t="s">
+        <v>91</v>
+      </c>
+      <c r="D41" t="s">
+        <v>135</v>
+      </c>
+      <c r="E41">
+        <v>74</v>
+      </c>
+      <c r="F41">
+        <v>70</v>
+      </c>
+      <c r="G41">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>39</v>
+      </c>
+      <c r="B42" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42" t="s">
+        <v>92</v>
+      </c>
+      <c r="D42" t="s">
+        <v>136</v>
+      </c>
+      <c r="E42">
+        <v>72</v>
+      </c>
+      <c r="F42">
+        <v>75</v>
+      </c>
+      <c r="G42">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>39</v>
+      </c>
+      <c r="B43" t="s">
+        <v>52</v>
+      </c>
+      <c r="C43" t="s">
+        <v>137</v>
+      </c>
+      <c r="D43" t="s">
+        <v>138</v>
+      </c>
+      <c r="E43">
+        <v>65</v>
+      </c>
+      <c r="F43">
+        <v>78</v>
+      </c>
+      <c r="G43">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>39</v>
+      </c>
+      <c r="B44" t="s">
+        <v>52</v>
+      </c>
+      <c r="C44" t="s">
+        <v>45</v>
+      </c>
+      <c r="D44" t="s">
+        <v>139</v>
+      </c>
+      <c r="E44">
+        <v>73</v>
+      </c>
+      <c r="F44">
+        <v>81</v>
+      </c>
+      <c r="G44">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>39</v>
+      </c>
+      <c r="B45" t="s">
+        <v>52</v>
+      </c>
+      <c r="C45" t="s">
+        <v>28</v>
+      </c>
+      <c r="D45" t="s">
+        <v>140</v>
+      </c>
+      <c r="E45">
+        <v>66</v>
+      </c>
+      <c r="F45">
+        <v>77</v>
+      </c>
+      <c r="G45">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>39</v>
+      </c>
+      <c r="B46" t="s">
+        <v>54</v>
+      </c>
+      <c r="C46" t="s">
+        <v>19</v>
+      </c>
+      <c r="D46" t="s">
+        <v>141</v>
+      </c>
+      <c r="E46">
+        <v>80</v>
+      </c>
+      <c r="F46">
+        <v>56</v>
+      </c>
+      <c r="G46">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>39</v>
+      </c>
+      <c r="B47" t="s">
+        <v>54</v>
+      </c>
+      <c r="C47" t="s">
+        <v>26</v>
+      </c>
+      <c r="D47" t="s">
+        <v>142</v>
+      </c>
+      <c r="E47">
+        <v>75</v>
+      </c>
+      <c r="F47">
+        <v>68</v>
+      </c>
+      <c r="G47">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>39</v>
+      </c>
+      <c r="B48" t="s">
+        <v>54</v>
+      </c>
+      <c r="C48" t="s">
+        <v>86</v>
+      </c>
+      <c r="D48" t="s">
+        <v>143</v>
+      </c>
+      <c r="E48">
+        <v>74</v>
+      </c>
+      <c r="F48">
+        <v>61</v>
+      </c>
+      <c r="G48">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>39</v>
+      </c>
+      <c r="B49" t="s">
+        <v>54</v>
+      </c>
+      <c r="C49" t="s">
+        <v>88</v>
+      </c>
+      <c r="D49" t="s">
+        <v>144</v>
+      </c>
+      <c r="E49">
+        <v>81</v>
+      </c>
+      <c r="F49">
+        <v>66</v>
+      </c>
+      <c r="G49">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>39</v>
+      </c>
+      <c r="B50" t="s">
+        <v>54</v>
+      </c>
+      <c r="C50" t="s">
+        <v>21</v>
+      </c>
+      <c r="D50" t="s">
+        <v>145</v>
+      </c>
+      <c r="E50">
+        <v>76</v>
+      </c>
+      <c r="F50">
+        <v>78</v>
+      </c>
+      <c r="G50">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>39</v>
+      </c>
+      <c r="B51" t="s">
+        <v>54</v>
+      </c>
+      <c r="C51" t="s">
+        <v>119</v>
+      </c>
+      <c r="D51" t="s">
+        <v>146</v>
+      </c>
+      <c r="E51">
+        <v>75</v>
+      </c>
+      <c r="F51">
+        <v>68</v>
+      </c>
+      <c r="G51">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>39</v>
+      </c>
+      <c r="B52" t="s">
+        <v>54</v>
+      </c>
+      <c r="C52" t="s">
+        <v>147</v>
+      </c>
+      <c r="D52" t="s">
+        <v>148</v>
+      </c>
+      <c r="E52">
+        <v>77</v>
+      </c>
+      <c r="F52">
+        <v>70</v>
+      </c>
+      <c r="G52">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>39</v>
+      </c>
+      <c r="B53" t="s">
+        <v>54</v>
+      </c>
+      <c r="C53" t="s">
+        <v>133</v>
+      </c>
+      <c r="D53" t="s">
+        <v>149</v>
+      </c>
+      <c r="E53">
+        <v>69</v>
+      </c>
+      <c r="F53">
+        <v>78</v>
+      </c>
+      <c r="G53">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>39</v>
+      </c>
+      <c r="B54" t="s">
+        <v>54</v>
+      </c>
+      <c r="C54" t="s">
+        <v>137</v>
+      </c>
+      <c r="D54" t="s">
+        <v>150</v>
+      </c>
+      <c r="E54">
+        <v>73</v>
+      </c>
+      <c r="F54">
+        <v>75</v>
+      </c>
+      <c r="G54">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>39</v>
+      </c>
+      <c r="B55" t="s">
+        <v>54</v>
+      </c>
+      <c r="C55" t="s">
+        <v>45</v>
+      </c>
+      <c r="D55" t="s">
+        <v>151</v>
+      </c>
+      <c r="E55">
+        <v>64</v>
+      </c>
+      <c r="F55">
+        <v>76</v>
+      </c>
+      <c r="G55">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>39</v>
+      </c>
+      <c r="B56" t="s">
+        <v>54</v>
+      </c>
+      <c r="C56" t="s">
+        <v>28</v>
+      </c>
+      <c r="D56" t="s">
+        <v>152</v>
+      </c>
+      <c r="E56">
+        <v>73</v>
+      </c>
+      <c r="F56">
+        <v>82</v>
+      </c>
+      <c r="G56">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>38</v>
+      </c>
+      <c r="B57" t="s">
+        <v>46</v>
+      </c>
+      <c r="C57" t="s">
+        <v>19</v>
+      </c>
+      <c r="D57" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="E57">
+        <v>81</v>
+      </c>
+      <c r="F57">
+        <v>50</v>
+      </c>
+      <c r="G57">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>38</v>
+      </c>
+      <c r="B58" t="s">
+        <v>46</v>
+      </c>
+      <c r="C58" t="s">
+        <v>21</v>
+      </c>
+      <c r="D58" t="s">
         <v>20</v>
       </c>
-      <c r="D2">
-        <v>81</v>
-      </c>
-      <c r="E2">
+      <c r="E58">
+        <v>71</v>
+      </c>
+      <c r="F58">
+        <v>65</v>
+      </c>
+      <c r="G58">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>38</v>
+      </c>
+      <c r="B59" t="s">
+        <v>46</v>
+      </c>
+      <c r="C59" t="s">
+        <v>23</v>
+      </c>
+      <c r="D59" t="s">
+        <v>22</v>
+      </c>
+      <c r="E59">
+        <v>60</v>
+      </c>
+      <c r="F59">
+        <v>75</v>
+      </c>
+      <c r="G59">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>38</v>
+      </c>
+      <c r="B60" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60" t="s">
+        <v>19</v>
+      </c>
+      <c r="D60" t="s">
+        <v>24</v>
+      </c>
+      <c r="E60">
+        <v>73</v>
+      </c>
+      <c r="F60">
         <v>50</v>
       </c>
-      <c r="F2">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3">
-        <v>71</v>
-      </c>
-      <c r="E3">
-        <v>65</v>
-      </c>
-      <c r="F3">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4">
+      <c r="G60">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>38</v>
+      </c>
+      <c r="B61" t="s">
+        <v>7</v>
+      </c>
+      <c r="C61" t="s">
+        <v>26</v>
+      </c>
+      <c r="D61" t="s">
+        <v>25</v>
+      </c>
+      <c r="E61">
+        <v>75</v>
+      </c>
+      <c r="F61">
+        <v>70</v>
+      </c>
+      <c r="G61">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>38</v>
+      </c>
+      <c r="B62" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62" t="s">
+        <v>28</v>
+      </c>
+      <c r="D62" t="s">
+        <v>27</v>
+      </c>
+      <c r="E62">
         <v>60</v>
       </c>
-      <c r="E4">
-        <v>75</v>
-      </c>
-      <c r="F4">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5">
-        <v>73</v>
-      </c>
-      <c r="E5">
-        <v>50</v>
-      </c>
-      <c r="F5">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6">
-        <v>75</v>
-      </c>
-      <c r="E6">
-        <v>70</v>
-      </c>
-      <c r="F6">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7">
-        <v>60</v>
-      </c>
-      <c r="E7">
+      <c r="F62">
         <v>86</v>
       </c>
-      <c r="F7">
+      <c r="G62">
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B63" t="s">
+        <v>42</v>
+      </c>
+      <c r="C63" t="s">
         <v>45</v>
       </c>
-      <c r="B8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8">
+      <c r="D63" t="s">
+        <v>44</v>
+      </c>
+      <c r="E63">
         <v>55</v>
       </c>
-      <c r="E8">
+      <c r="F63">
         <v>74</v>
       </c>
-      <c r="F8">
+      <c r="G63">
         <v>74</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1011,8 +2895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1023,15 +2907,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1039,7 +2923,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1047,7 +2931,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -1055,7 +2939,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5">
         <v>2</v>

</xml_diff>

<commit_message>
More squad updates in test data
</commit_message>
<xml_diff>
--- a/Source/EuroManager.WorldSimulator.Tests.Manual/Data.xlsx
+++ b/Source/EuroManager.WorldSimulator.Tests.Manual/Data.xlsx
@@ -2438,8 +2438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G353"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A324" workbookViewId="0">
-      <selection activeCell="C347" sqref="C347"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A146" workbookViewId="0">
+      <selection activeCell="G178" sqref="G178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2629,10 +2629,10 @@
         <v>70</v>
       </c>
       <c r="F8">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G8">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -2655,7 +2655,7 @@
         <v>84</v>
       </c>
       <c r="G9">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -2678,7 +2678,7 @@
         <v>81</v>
       </c>
       <c r="G10">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -4265,7 +4265,7 @@
         <v>54</v>
       </c>
       <c r="G79">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
@@ -4305,13 +4305,13 @@
         <v>161</v>
       </c>
       <c r="E81">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F81">
         <v>75</v>
       </c>
       <c r="G81">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
@@ -4328,13 +4328,13 @@
         <v>193</v>
       </c>
       <c r="E82">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F82">
         <v>74</v>
       </c>
       <c r="G82">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
@@ -4449,7 +4449,7 @@
         <v>82</v>
       </c>
       <c r="G87">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
@@ -4518,7 +4518,7 @@
         <v>63</v>
       </c>
       <c r="G90">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
@@ -4541,7 +4541,7 @@
         <v>68</v>
       </c>
       <c r="G91">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
@@ -4633,7 +4633,7 @@
         <v>81</v>
       </c>
       <c r="G95">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
@@ -4656,7 +4656,7 @@
         <v>81</v>
       </c>
       <c r="G96">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
@@ -4679,7 +4679,7 @@
         <v>65</v>
       </c>
       <c r="G97">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
@@ -5507,7 +5507,7 @@
         <v>77</v>
       </c>
       <c r="G133">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.3">
@@ -6358,7 +6358,7 @@
         <v>54</v>
       </c>
       <c r="G170">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.3">
@@ -6404,7 +6404,7 @@
         <v>75</v>
       </c>
       <c r="G172">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.3">
@@ -6447,10 +6447,10 @@
         <v>61</v>
       </c>
       <c r="F174">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G174">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.3">
@@ -6470,7 +6470,7 @@
         <v>53</v>
       </c>
       <c r="F175">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G175">
         <v>84</v>
@@ -6519,7 +6519,7 @@
         <v>76</v>
       </c>
       <c r="G177">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>